<commit_message>
Adaption of script and datafiles to run ODYM for Ind
</commit_message>
<xml_diff>
--- a/Data/4_EI_ProcessEnergyIntensity_V2.1.xlsx
+++ b/Data/4_EI_ProcessEnergyIntensity_V2.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13695" windowHeight="5378" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13692" windowHeight="5376" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="log" sheetId="6" r:id="rId4"/>
     <sheet name="ref" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -98,9 +98,6 @@
     <t># Two types are supported: list and table</t>
   </si>
   <si>
-    <t>SSP_Regions_32</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -369,13 +366,16 @@
   </si>
   <si>
     <t>From ecoinvent scenario generator, responsible: Niko Heeren. At the moment, energy us is not extracted separately. No data here in this parameter.</t>
+  </si>
+  <si>
+    <t>300 - 400 kWh per tonne of copper // 350 chosen  Schlesinger (2011) Extractive metallurgy of copper. Converted into MJ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -408,6 +408,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -442,7 +448,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -474,9 +480,12 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -492,7 +501,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -781,39 +790,39 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.1328125" customWidth="1"/>
-    <col min="3" max="3" width="23.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="41" customWidth="1"/>
     <col min="5" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.53125" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" customWidth="1"/>
     <col min="8" max="8" width="43" customWidth="1"/>
-    <col min="9" max="9" width="3.46484375" customWidth="1"/>
+    <col min="9" max="9" width="3.44140625" customWidth="1"/>
     <col min="10" max="11" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>24</v>
@@ -823,12 +832,12 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
@@ -838,12 +847,12 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
@@ -853,57 +862,57 @@
       </c>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
@@ -913,27 +922,27 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>24</v>
@@ -943,7 +952,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -958,7 +967,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -973,7 +982,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -988,12 +997,12 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>24</v>
@@ -1003,12 +1012,12 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>24</v>
@@ -1018,60 +1027,60 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="E16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="E17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="E18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="E19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="11"/>
       <c r="C20" s="11"/>
       <c r="E20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="19">
         <v>13</v>
@@ -1084,18 +1093,18 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>24</v>
@@ -1105,18 +1114,18 @@
       <c r="H22" s="9"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>24</v>
@@ -1124,22 +1133,22 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="H23" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="C24" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>24</v>
@@ -1147,22 +1156,22 @@
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>62</v>
-      </c>
       <c r="C25" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>24</v>
@@ -1170,22 +1179,22 @@
       <c r="F25" s="9"/>
       <c r="G25" s="9"/>
       <c r="H25" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>87</v>
-      </c>
       <c r="C26" s="15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>24</v>
@@ -1193,11 +1202,11 @@
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1208,7 +1217,7 @@
       <c r="K27" s="11"/>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E28" s="1" t="s">
         <v>24</v>
       </c>
@@ -1219,7 +1228,7 @@
       <c r="K28" s="11"/>
       <c r="L28" s="12"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E29" s="1" t="s">
         <v>24</v>
       </c>
@@ -1230,7 +1239,7 @@
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E30" s="1" t="s">
         <v>24</v>
       </c>
@@ -1241,7 +1250,7 @@
       <c r="K30" s="11"/>
       <c r="L30" s="11"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E31" s="1" t="s">
         <v>24</v>
       </c>
@@ -1252,7 +1261,7 @@
       <c r="K31" s="11"/>
       <c r="L31" s="11"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E32" s="1" t="s">
         <v>24</v>
       </c>
@@ -1263,7 +1272,7 @@
       <c r="K32" s="11"/>
       <c r="L32" s="11"/>
     </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E33" s="5"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
@@ -1273,7 +1282,7 @@
       <c r="K33" s="11"/>
       <c r="L33" s="11"/>
     </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
       <c r="G34" s="11"/>
@@ -1283,7 +1292,7 @@
       <c r="K34" s="11"/>
       <c r="L34" s="11"/>
     </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
@@ -1293,7 +1302,7 @@
       <c r="K35" s="11"/>
       <c r="L35" s="11"/>
     </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="5:12" x14ac:dyDescent="0.3">
       <c r="E36" s="11"/>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
@@ -1313,461 +1322,466 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N481"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="54.53125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.19921875" customWidth="1"/>
-    <col min="3" max="3" width="30.46484375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.21875" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.46484375" customWidth="1"/>
-    <col min="7" max="7" width="22.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2">
         <v>2010</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
       <c r="F2" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="C3">
         <v>2010</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="C4">
         <v>2010</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="C5">
         <v>2010</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="C6">
         <v>2010</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <v>2010</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
       <c r="F7" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C8">
         <v>2010</v>
       </c>
       <c r="D8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1260</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9">
         <v>2010</v>
       </c>
       <c r="D9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>2010</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C11">
         <v>2010</v>
       </c>
       <c r="D11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12">
         <v>2010</v>
       </c>
       <c r="D12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C13">
         <v>2010</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>2010</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+      <c r="D21" s="27"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+      <c r="D22" s="27"/>
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+      <c r="D23" s="27"/>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+      <c r="D24" s="27"/>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.3">
+      <c r="D25" s="27"/>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I27" s="9"/>
       <c r="J27" s="9"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="I28" s="9"/>
       <c r="J28" s="9"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="23"/>
       <c r="B29" s="9"/>
       <c r="C29" s="21"/>
@@ -1776,7 +1790,7 @@
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="23"/>
       <c r="B30" s="9"/>
       <c r="C30" s="8"/>
@@ -1786,7 +1800,7 @@
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="23"/>
       <c r="B31" s="9"/>
       <c r="C31" s="8"/>
@@ -1796,7 +1810,7 @@
       <c r="J31" s="9"/>
       <c r="M31" s="9"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="23"/>
       <c r="B32" s="9"/>
       <c r="C32" s="8"/>
@@ -1807,14 +1821,14 @@
       <c r="J32" s="9"/>
       <c r="M32" s="9"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F33" s="9"/>
       <c r="G33" s="9"/>
       <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="M33" s="9"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -1823,7 +1837,7 @@
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F35" s="9"/>
       <c r="G35" s="9"/>
       <c r="I35" s="9"/>
@@ -1831,7 +1845,7 @@
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F36" s="9"/>
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
@@ -1840,7 +1854,7 @@
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
       <c r="I37" s="9"/>
@@ -1848,7 +1862,7 @@
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="23"/>
       <c r="B38" s="9"/>
       <c r="C38" s="8"/>
@@ -1860,7 +1874,7 @@
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="23"/>
       <c r="B39" s="9"/>
       <c r="C39" s="8"/>
@@ -1871,7 +1885,7 @@
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="23"/>
       <c r="B40" s="9"/>
       <c r="C40" s="8"/>
@@ -1883,7 +1897,7 @@
       <c r="K40" s="9"/>
       <c r="N40" s="9"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="23"/>
       <c r="B41" s="9"/>
       <c r="C41" s="8"/>
@@ -1894,7 +1908,7 @@
       <c r="K41" s="9"/>
       <c r="N41" s="9"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="23"/>
       <c r="B42" s="9"/>
       <c r="C42" s="8"/>
@@ -1906,7 +1920,7 @@
       <c r="K42" s="9"/>
       <c r="N42" s="9"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="23"/>
       <c r="B43" s="9"/>
       <c r="C43" s="8"/>
@@ -1917,7 +1931,7 @@
       <c r="K43" s="9"/>
       <c r="N43" s="9"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="23"/>
       <c r="B44" s="9"/>
       <c r="C44" s="8"/>
@@ -1929,7 +1943,7 @@
       <c r="K44" s="9"/>
       <c r="N44" s="9"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="23"/>
       <c r="B45" s="9"/>
       <c r="C45" s="8"/>
@@ -1940,7 +1954,7 @@
       <c r="K45" s="9"/>
       <c r="N45" s="9"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="23"/>
       <c r="B46" s="9"/>
       <c r="C46" s="8"/>
@@ -1952,7 +1966,7 @@
       <c r="K46" s="9"/>
       <c r="N46" s="9"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="23"/>
       <c r="B47" s="9"/>
       <c r="C47" s="8"/>
@@ -1963,7 +1977,7 @@
       <c r="K47" s="9"/>
       <c r="N47" s="9"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="23"/>
       <c r="B48" s="9"/>
       <c r="C48" s="8"/>
@@ -1975,7 +1989,7 @@
       <c r="K48" s="9"/>
       <c r="N48" s="9"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="23"/>
       <c r="B49" s="9"/>
       <c r="C49" s="8"/>
@@ -1986,7 +2000,7 @@
       <c r="K49" s="9"/>
       <c r="N49" s="9"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="23"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
@@ -1998,7 +2012,7 @@
       <c r="K50" s="9"/>
       <c r="N50" s="9"/>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="23"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
@@ -2008,7 +2022,7 @@
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="23"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
@@ -2019,7 +2033,7 @@
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="23"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
@@ -2029,7 +2043,7 @@
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="23"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
@@ -2040,7 +2054,7 @@
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="23"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
@@ -2050,7 +2064,7 @@
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="23"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
@@ -2061,7 +2075,7 @@
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="23"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -2071,7 +2085,7 @@
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="23"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
@@ -2082,7 +2096,7 @@
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="23"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
@@ -2092,7 +2106,7 @@
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="23"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
@@ -2103,7 +2117,7 @@
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="23"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
@@ -2113,7 +2127,7 @@
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="23"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
@@ -2124,7 +2138,7 @@
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="23"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
@@ -2134,7 +2148,7 @@
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="23"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
@@ -2145,7 +2159,7 @@
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="23"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
@@ -2155,7 +2169,7 @@
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="23"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
@@ -2165,7 +2179,7 @@
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="23"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
@@ -2174,7 +2188,7 @@
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="23"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
@@ -2184,7 +2198,7 @@
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="23"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
@@ -2193,7 +2207,7 @@
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="23"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
@@ -2203,7 +2217,7 @@
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="23"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
@@ -2212,7 +2226,7 @@
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="23"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
@@ -2222,7 +2236,7 @@
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="23"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
@@ -2231,7 +2245,7 @@
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="23"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
@@ -2241,7 +2255,7 @@
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="23"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
@@ -2250,7 +2264,7 @@
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="23"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
@@ -2260,7 +2274,7 @@
       <c r="I76" s="9"/>
       <c r="J76" s="9"/>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="23"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
@@ -2269,7 +2283,7 @@
       <c r="I77" s="9"/>
       <c r="J77" s="9"/>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A78" s="23"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
@@ -2279,7 +2293,7 @@
       <c r="I78" s="9"/>
       <c r="J78" s="9"/>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A79" s="23"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
@@ -2288,7 +2302,7 @@
       <c r="I79" s="9"/>
       <c r="J79" s="9"/>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="23"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
@@ -2298,7 +2312,7 @@
       <c r="I80" s="9"/>
       <c r="J80" s="9"/>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" s="23"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
@@ -2307,7 +2321,7 @@
       <c r="I81" s="9"/>
       <c r="J81" s="9"/>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" s="23"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
@@ -2317,7 +2331,7 @@
       <c r="I82" s="9"/>
       <c r="J82" s="9"/>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" s="23"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
@@ -2326,7 +2340,7 @@
       <c r="I83" s="9"/>
       <c r="J83" s="9"/>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" s="23"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
@@ -2336,7 +2350,7 @@
       <c r="I84" s="9"/>
       <c r="J84" s="9"/>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" s="23"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
@@ -2345,7 +2359,7 @@
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" s="23"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
@@ -2355,7 +2369,7 @@
       <c r="I86" s="9"/>
       <c r="J86" s="9"/>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A87" s="23"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
@@ -2364,7 +2378,7 @@
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A88" s="23"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
@@ -2374,7 +2388,7 @@
       <c r="I88" s="9"/>
       <c r="J88" s="9"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A89" s="23"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
@@ -2383,7 +2397,7 @@
       <c r="I89" s="9"/>
       <c r="J89" s="9"/>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A90" s="23"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
@@ -2393,7 +2407,7 @@
       <c r="I90" s="9"/>
       <c r="J90" s="9"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A91" s="23"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
@@ -2402,7 +2416,7 @@
       <c r="I91" s="9"/>
       <c r="J91" s="9"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A92" s="23"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
@@ -2412,7 +2426,7 @@
       <c r="I92" s="9"/>
       <c r="J92" s="9"/>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A93" s="23"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
@@ -2421,7 +2435,7 @@
       <c r="I93" s="9"/>
       <c r="J93" s="9"/>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A94" s="23"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
@@ -2431,7 +2445,7 @@
       <c r="I94" s="9"/>
       <c r="J94" s="9"/>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A95" s="23"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -2440,7 +2454,7 @@
       <c r="I95" s="9"/>
       <c r="J95" s="9"/>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A96" s="23"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
@@ -2450,7 +2464,7 @@
       <c r="I96" s="9"/>
       <c r="J96" s="9"/>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A97" s="23"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
@@ -2459,7 +2473,7 @@
       <c r="I97" s="9"/>
       <c r="J97" s="9"/>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A98" s="23"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
@@ -2469,7 +2483,7 @@
       <c r="I98" s="9"/>
       <c r="J98" s="9"/>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A99" s="23"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
@@ -2478,7 +2492,7 @@
       <c r="I99" s="9"/>
       <c r="J99" s="9"/>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A100" s="23"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
@@ -2488,7 +2502,7 @@
       <c r="I100" s="9"/>
       <c r="J100" s="9"/>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A101" s="23"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
@@ -2497,7 +2511,7 @@
       <c r="I101" s="9"/>
       <c r="J101" s="9"/>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A102" s="23"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
@@ -2507,7 +2521,7 @@
       <c r="I102" s="9"/>
       <c r="J102" s="9"/>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A103" s="23"/>
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
@@ -2516,7 +2530,7 @@
       <c r="I103" s="9"/>
       <c r="J103" s="9"/>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A104" s="23"/>
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
@@ -2526,7 +2540,7 @@
       <c r="I104" s="9"/>
       <c r="J104" s="9"/>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A105" s="23"/>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
@@ -2535,7 +2549,7 @@
       <c r="I105" s="9"/>
       <c r="J105" s="9"/>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A106" s="23"/>
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
@@ -2545,7 +2559,7 @@
       <c r="I106" s="9"/>
       <c r="J106" s="9"/>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A107" s="23"/>
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
@@ -2554,7 +2568,7 @@
       <c r="I107" s="9"/>
       <c r="J107" s="9"/>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A108" s="23"/>
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
@@ -2564,7 +2578,7 @@
       <c r="I108" s="9"/>
       <c r="J108" s="9"/>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A109" s="23"/>
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
@@ -2573,7 +2587,7 @@
       <c r="I109" s="9"/>
       <c r="J109" s="9"/>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A110" s="23"/>
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
@@ -2583,7 +2597,7 @@
       <c r="I110" s="9"/>
       <c r="J110" s="9"/>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A111" s="23"/>
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
@@ -2592,7 +2606,7 @@
       <c r="I111" s="9"/>
       <c r="J111" s="9"/>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A112" s="23"/>
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
@@ -2602,7 +2616,7 @@
       <c r="I112" s="9"/>
       <c r="J112" s="9"/>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A113" s="23"/>
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
@@ -2611,7 +2625,7 @@
       <c r="I113" s="9"/>
       <c r="J113" s="9"/>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A114" s="23"/>
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
@@ -2621,7 +2635,7 @@
       <c r="I114" s="9"/>
       <c r="J114" s="9"/>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A115" s="23"/>
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
@@ -2630,7 +2644,7 @@
       <c r="I115" s="9"/>
       <c r="J115" s="9"/>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A116" s="23"/>
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
@@ -2640,7 +2654,7 @@
       <c r="I116" s="9"/>
       <c r="J116" s="9"/>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A117" s="23"/>
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
@@ -2649,7 +2663,7 @@
       <c r="I117" s="9"/>
       <c r="J117" s="9"/>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A118" s="23"/>
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
@@ -2659,7 +2673,7 @@
       <c r="I118" s="9"/>
       <c r="J118" s="9"/>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="23"/>
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
@@ -2668,7 +2682,7 @@
       <c r="I119" s="9"/>
       <c r="J119" s="9"/>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" s="23"/>
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
@@ -2678,7 +2692,7 @@
       <c r="I120" s="9"/>
       <c r="J120" s="9"/>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" s="23"/>
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
@@ -2687,1281 +2701,1281 @@
       <c r="I121" s="9"/>
       <c r="J121" s="9"/>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B122" s="9"/>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B123" s="9"/>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B124" s="9"/>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B125" s="9"/>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B126" s="9"/>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B127" s="9"/>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B128" s="9"/>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="129" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B129" s="9"/>
       <c r="E129" s="9"/>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="130" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B130" s="9"/>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="131" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B131" s="9"/>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="132" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B132" s="9"/>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="133" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B133" s="9"/>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="134" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B134" s="9"/>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="135" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B135" s="9"/>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="136" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B136" s="9"/>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="137" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B137" s="9"/>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="138" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B138" s="9"/>
     </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="139" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B139" s="9"/>
     </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="140" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B140" s="9"/>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="141" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B141" s="9"/>
     </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="142" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B142" s="9"/>
     </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="143" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B143" s="9"/>
     </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="144" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B144" s="9"/>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B145" s="9"/>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B146" s="9"/>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B147" s="9"/>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B148" s="9"/>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B149" s="9"/>
     </row>
-    <row r="150" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B150" s="9"/>
     </row>
-    <row r="151" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="151" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B151" s="9"/>
     </row>
-    <row r="152" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B152" s="9"/>
     </row>
-    <row r="153" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B153" s="9"/>
     </row>
-    <row r="154" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="154" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B154" s="9"/>
     </row>
-    <row r="155" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="155" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B155" s="9"/>
     </row>
-    <row r="156" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="156" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B156" s="9"/>
     </row>
-    <row r="157" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="157" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B157" s="9"/>
     </row>
-    <row r="158" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="158" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B158" s="9"/>
     </row>
-    <row r="159" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="159" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B159" s="9"/>
     </row>
-    <row r="160" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="160" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B160" s="9"/>
     </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B161" s="9"/>
       <c r="E161" s="9"/>
     </row>
-    <row r="162" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="162" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B162" s="9"/>
     </row>
-    <row r="163" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="163" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B163" s="9"/>
     </row>
-    <row r="164" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="164" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B164" s="9"/>
     </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="165" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B165" s="9"/>
     </row>
-    <row r="166" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="166" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B166" s="9"/>
     </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="167" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B167" s="9"/>
     </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="168" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B168" s="9"/>
     </row>
-    <row r="169" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="169" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B169" s="9"/>
     </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="170" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B170" s="9"/>
     </row>
-    <row r="171" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="171" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B171" s="9"/>
     </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="172" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B172" s="9"/>
     </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="173" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B173" s="9"/>
     </row>
-    <row r="174" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="174" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B174" s="9"/>
     </row>
-    <row r="175" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="175" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B175" s="9"/>
     </row>
-    <row r="176" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="176" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B176" s="9"/>
     </row>
-    <row r="177" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="177" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B177" s="9"/>
     </row>
-    <row r="178" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="178" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B178" s="9"/>
     </row>
-    <row r="179" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="179" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B179" s="9"/>
     </row>
-    <row r="180" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="180" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B180" s="9"/>
     </row>
-    <row r="181" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="181" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B181" s="9"/>
     </row>
-    <row r="182" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="182" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B182" s="9"/>
     </row>
-    <row r="183" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="183" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B183" s="9"/>
     </row>
-    <row r="184" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="184" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B184" s="9"/>
     </row>
-    <row r="185" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="185" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B185" s="9"/>
     </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="186" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B186" s="9"/>
     </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="187" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B187" s="9"/>
     </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="188" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B188" s="9"/>
     </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="189" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B189" s="9"/>
     </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="190" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B190" s="9"/>
     </row>
-    <row r="191" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="191" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B191" s="9"/>
     </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="192" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B192" s="9"/>
     </row>
-    <row r="193" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="193" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B193" s="9"/>
       <c r="E193" s="9"/>
     </row>
-    <row r="194" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="194" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B194" s="9"/>
     </row>
-    <row r="195" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="195" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B195" s="9"/>
     </row>
-    <row r="196" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="196" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B196" s="9"/>
     </row>
-    <row r="197" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="197" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B197" s="9"/>
     </row>
-    <row r="198" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="198" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B198" s="9"/>
     </row>
-    <row r="199" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="199" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B199" s="9"/>
     </row>
-    <row r="200" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="200" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B200" s="9"/>
     </row>
-    <row r="201" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="201" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B201" s="9"/>
     </row>
-    <row r="202" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="202" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B202" s="9"/>
     </row>
-    <row r="203" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="203" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B203" s="9"/>
     </row>
-    <row r="204" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="204" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B204" s="9"/>
     </row>
-    <row r="205" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="205" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B205" s="9"/>
     </row>
-    <row r="206" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="206" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B206" s="9"/>
     </row>
-    <row r="207" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="207" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B207" s="9"/>
     </row>
-    <row r="208" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="208" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B208" s="9"/>
     </row>
-    <row r="209" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="209" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B209" s="9"/>
     </row>
-    <row r="210" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="210" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B210" s="9"/>
     </row>
-    <row r="211" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="211" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B211" s="9"/>
     </row>
-    <row r="212" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="212" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B212" s="9"/>
     </row>
-    <row r="213" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="213" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B213" s="9"/>
     </row>
-    <row r="214" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="214" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B214" s="9"/>
     </row>
-    <row r="215" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="215" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B215" s="9"/>
     </row>
-    <row r="216" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="216" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B216" s="9"/>
     </row>
-    <row r="217" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="217" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B217" s="9"/>
     </row>
-    <row r="218" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="218" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B218" s="9"/>
     </row>
-    <row r="219" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="219" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B219" s="9"/>
     </row>
-    <row r="220" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="220" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B220" s="9"/>
     </row>
-    <row r="221" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="221" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B221" s="9"/>
     </row>
-    <row r="222" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="222" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B222" s="9"/>
     </row>
-    <row r="223" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="223" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B223" s="9"/>
     </row>
-    <row r="224" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="224" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B224" s="9"/>
     </row>
-    <row r="225" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="225" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B225" s="9"/>
       <c r="E225" s="9"/>
     </row>
-    <row r="226" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="226" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B226" s="9"/>
     </row>
-    <row r="227" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="227" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B227" s="9"/>
     </row>
-    <row r="228" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="228" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B228" s="9"/>
     </row>
-    <row r="229" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="229" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B229" s="9"/>
     </row>
-    <row r="230" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="230" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B230" s="9"/>
     </row>
-    <row r="231" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="231" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B231" s="9"/>
     </row>
-    <row r="232" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="232" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B232" s="9"/>
     </row>
-    <row r="233" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="233" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B233" s="9"/>
     </row>
-    <row r="234" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="234" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B234" s="9"/>
     </row>
-    <row r="235" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="235" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B235" s="9"/>
     </row>
-    <row r="236" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="236" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B236" s="9"/>
     </row>
-    <row r="237" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="237" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B237" s="9"/>
     </row>
-    <row r="238" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="238" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B238" s="9"/>
     </row>
-    <row r="239" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="239" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B239" s="9"/>
     </row>
-    <row r="240" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="240" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B240" s="9"/>
     </row>
-    <row r="241" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="241" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B241" s="9"/>
     </row>
-    <row r="242" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="242" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B242" s="9"/>
     </row>
-    <row r="243" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="243" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B243" s="9"/>
     </row>
-    <row r="244" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="244" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B244" s="9"/>
     </row>
-    <row r="245" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="245" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B245" s="9"/>
     </row>
-    <row r="246" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="246" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B246" s="9"/>
     </row>
-    <row r="247" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="247" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B247" s="9"/>
     </row>
-    <row r="248" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="248" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B248" s="9"/>
     </row>
-    <row r="249" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="249" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B249" s="9"/>
     </row>
-    <row r="250" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="250" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B250" s="9"/>
     </row>
-    <row r="251" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="251" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B251" s="9"/>
     </row>
-    <row r="252" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="252" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B252" s="9"/>
     </row>
-    <row r="253" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="253" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B253" s="9"/>
     </row>
-    <row r="254" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="254" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B254" s="9"/>
     </row>
-    <row r="255" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="255" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B255" s="9"/>
     </row>
-    <row r="256" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="256" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B256" s="9"/>
     </row>
-    <row r="257" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="257" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B257" s="9"/>
       <c r="E257" s="9"/>
     </row>
-    <row r="258" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="258" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B258" s="9"/>
     </row>
-    <row r="259" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="259" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B259" s="9"/>
     </row>
-    <row r="260" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="260" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B260" s="9"/>
     </row>
-    <row r="261" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="261" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B261" s="9"/>
     </row>
-    <row r="262" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="262" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B262" s="9"/>
     </row>
-    <row r="263" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="263" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B263" s="9"/>
     </row>
-    <row r="264" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="264" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B264" s="9"/>
     </row>
-    <row r="265" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="265" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B265" s="9"/>
     </row>
-    <row r="266" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="266" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B266" s="9"/>
     </row>
-    <row r="267" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="267" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B267" s="9"/>
     </row>
-    <row r="268" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="268" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B268" s="9"/>
     </row>
-    <row r="269" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="269" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B269" s="9"/>
     </row>
-    <row r="270" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="270" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B270" s="9"/>
     </row>
-    <row r="271" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="271" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B271" s="9"/>
     </row>
-    <row r="272" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="272" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B272" s="9"/>
     </row>
-    <row r="273" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="273" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B273" s="9"/>
     </row>
-    <row r="274" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="274" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B274" s="9"/>
     </row>
-    <row r="275" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="275" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B275" s="9"/>
     </row>
-    <row r="276" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="276" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B276" s="9"/>
     </row>
-    <row r="277" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="277" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B277" s="9"/>
     </row>
-    <row r="278" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="278" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B278" s="9"/>
     </row>
-    <row r="279" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="279" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B279" s="9"/>
     </row>
-    <row r="280" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="280" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B280" s="9"/>
     </row>
-    <row r="281" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="281" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B281" s="9"/>
     </row>
-    <row r="282" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="282" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B282" s="9"/>
     </row>
-    <row r="283" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="283" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B283" s="9"/>
     </row>
-    <row r="284" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="284" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B284" s="9"/>
     </row>
-    <row r="285" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="285" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B285" s="9"/>
     </row>
-    <row r="286" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="286" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B286" s="9"/>
     </row>
-    <row r="287" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="287" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B287" s="9"/>
     </row>
-    <row r="288" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="288" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B288" s="9"/>
     </row>
-    <row r="289" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="289" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B289" s="9"/>
       <c r="E289" s="9"/>
     </row>
-    <row r="290" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="290" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B290" s="9"/>
       <c r="E290" s="9"/>
     </row>
-    <row r="291" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="291" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B291" s="9"/>
       <c r="E291" s="9"/>
     </row>
-    <row r="292" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="292" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B292" s="9"/>
       <c r="E292" s="9"/>
     </row>
-    <row r="293" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="293" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B293" s="9"/>
       <c r="E293" s="9"/>
     </row>
-    <row r="294" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="294" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B294" s="9"/>
       <c r="E294" s="9"/>
     </row>
-    <row r="295" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="295" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B295" s="9"/>
       <c r="E295" s="9"/>
     </row>
-    <row r="296" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="296" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B296" s="9"/>
       <c r="E296" s="9"/>
     </row>
-    <row r="297" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="297" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B297" s="9"/>
       <c r="E297" s="9"/>
     </row>
-    <row r="298" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="298" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B298" s="9"/>
       <c r="E298" s="9"/>
     </row>
-    <row r="299" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="299" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B299" s="9"/>
       <c r="E299" s="9"/>
     </row>
-    <row r="300" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="300" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B300" s="9"/>
       <c r="E300" s="9"/>
     </row>
-    <row r="301" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="301" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B301" s="9"/>
       <c r="E301" s="9"/>
     </row>
-    <row r="302" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="302" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B302" s="9"/>
       <c r="E302" s="9"/>
     </row>
-    <row r="303" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="303" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B303" s="9"/>
       <c r="E303" s="9"/>
     </row>
-    <row r="304" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="304" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B304" s="9"/>
       <c r="E304" s="9"/>
     </row>
-    <row r="305" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="305" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B305" s="9"/>
       <c r="E305" s="9"/>
     </row>
-    <row r="306" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="306" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B306" s="9"/>
       <c r="E306" s="9"/>
     </row>
-    <row r="307" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="307" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B307" s="9"/>
       <c r="E307" s="9"/>
     </row>
-    <row r="308" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="308" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B308" s="9"/>
       <c r="E308" s="9"/>
     </row>
-    <row r="309" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="309" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B309" s="9"/>
       <c r="E309" s="9"/>
     </row>
-    <row r="310" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="310" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B310" s="9"/>
       <c r="E310" s="9"/>
     </row>
-    <row r="311" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="311" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B311" s="9"/>
       <c r="E311" s="9"/>
     </row>
-    <row r="312" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="312" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B312" s="9"/>
       <c r="E312" s="9"/>
     </row>
-    <row r="313" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="313" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B313" s="9"/>
       <c r="E313" s="9"/>
     </row>
-    <row r="314" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="314" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B314" s="9"/>
       <c r="E314" s="9"/>
     </row>
-    <row r="315" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="315" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B315" s="9"/>
       <c r="E315" s="9"/>
     </row>
-    <row r="316" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="316" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B316" s="9"/>
       <c r="E316" s="9"/>
     </row>
-    <row r="317" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="317" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B317" s="9"/>
       <c r="E317" s="9"/>
     </row>
-    <row r="318" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="318" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B318" s="9"/>
       <c r="E318" s="9"/>
     </row>
-    <row r="319" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="319" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B319" s="9"/>
       <c r="E319" s="9"/>
     </row>
-    <row r="320" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="320" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B320" s="9"/>
       <c r="E320" s="9"/>
     </row>
-    <row r="321" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="321" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B321" s="9"/>
       <c r="E321" s="9"/>
     </row>
-    <row r="322" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="322" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B322" s="9"/>
       <c r="E322" s="9"/>
     </row>
-    <row r="323" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="323" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B323" s="9"/>
       <c r="E323" s="9"/>
     </row>
-    <row r="324" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="324" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B324" s="9"/>
       <c r="E324" s="9"/>
     </row>
-    <row r="325" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="325" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B325" s="9"/>
       <c r="E325" s="9"/>
     </row>
-    <row r="326" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="326" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B326" s="9"/>
       <c r="E326" s="9"/>
     </row>
-    <row r="327" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="327" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B327" s="9"/>
       <c r="E327" s="9"/>
     </row>
-    <row r="328" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="328" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B328" s="9"/>
       <c r="E328" s="9"/>
     </row>
-    <row r="329" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="329" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B329" s="9"/>
       <c r="E329" s="9"/>
     </row>
-    <row r="330" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="330" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B330" s="9"/>
       <c r="E330" s="9"/>
     </row>
-    <row r="331" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="331" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B331" s="9"/>
       <c r="E331" s="9"/>
     </row>
-    <row r="332" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="332" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B332" s="9"/>
       <c r="E332" s="9"/>
     </row>
-    <row r="333" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="333" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B333" s="9"/>
       <c r="E333" s="9"/>
     </row>
-    <row r="334" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="334" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B334" s="9"/>
       <c r="E334" s="9"/>
     </row>
-    <row r="335" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="335" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B335" s="9"/>
       <c r="E335" s="9"/>
     </row>
-    <row r="336" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="336" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B336" s="9"/>
       <c r="E336" s="9"/>
     </row>
-    <row r="337" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="337" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B337" s="9"/>
       <c r="E337" s="9"/>
     </row>
-    <row r="338" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="338" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B338" s="9"/>
       <c r="E338" s="9"/>
     </row>
-    <row r="339" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="339" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B339" s="9"/>
       <c r="E339" s="9"/>
     </row>
-    <row r="340" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="340" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B340" s="9"/>
       <c r="E340" s="9"/>
     </row>
-    <row r="341" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="341" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B341" s="9"/>
       <c r="E341" s="9"/>
     </row>
-    <row r="342" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="342" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B342" s="9"/>
       <c r="E342" s="9"/>
     </row>
-    <row r="343" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="343" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B343" s="9"/>
       <c r="E343" s="9"/>
     </row>
-    <row r="344" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="344" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B344" s="9"/>
       <c r="E344" s="9"/>
     </row>
-    <row r="345" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="345" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B345" s="9"/>
       <c r="E345" s="9"/>
     </row>
-    <row r="346" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="346" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B346" s="9"/>
       <c r="E346" s="9"/>
     </row>
-    <row r="347" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="347" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B347" s="9"/>
       <c r="E347" s="9"/>
     </row>
-    <row r="348" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="348" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B348" s="9"/>
       <c r="E348" s="9"/>
     </row>
-    <row r="349" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="349" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B349" s="9"/>
       <c r="E349" s="9"/>
     </row>
-    <row r="350" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="350" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B350" s="9"/>
       <c r="E350" s="9"/>
     </row>
-    <row r="351" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="351" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B351" s="9"/>
       <c r="E351" s="9"/>
     </row>
-    <row r="352" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="352" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B352" s="9"/>
       <c r="E352" s="9"/>
     </row>
-    <row r="353" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="353" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B353" s="9"/>
       <c r="E353" s="9"/>
     </row>
-    <row r="354" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="354" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B354" s="9"/>
       <c r="E354" s="9"/>
     </row>
-    <row r="355" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="355" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B355" s="9"/>
       <c r="E355" s="9"/>
     </row>
-    <row r="356" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="356" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B356" s="9"/>
       <c r="E356" s="9"/>
     </row>
-    <row r="357" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="357" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B357" s="9"/>
       <c r="E357" s="9"/>
     </row>
-    <row r="358" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="358" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B358" s="9"/>
       <c r="E358" s="9"/>
     </row>
-    <row r="359" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="359" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B359" s="9"/>
       <c r="E359" s="9"/>
     </row>
-    <row r="360" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="360" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B360" s="9"/>
       <c r="E360" s="9"/>
     </row>
-    <row r="361" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="361" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B361" s="9"/>
       <c r="E361" s="9"/>
     </row>
-    <row r="362" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="362" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B362" s="9"/>
       <c r="E362" s="9"/>
     </row>
-    <row r="363" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="363" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B363" s="9"/>
       <c r="E363" s="9"/>
     </row>
-    <row r="364" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="364" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B364" s="9"/>
       <c r="E364" s="9"/>
     </row>
-    <row r="365" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="365" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B365" s="9"/>
       <c r="E365" s="9"/>
     </row>
-    <row r="366" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="366" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B366" s="9"/>
       <c r="E366" s="9"/>
     </row>
-    <row r="367" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="367" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B367" s="9"/>
       <c r="E367" s="9"/>
     </row>
-    <row r="368" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="368" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B368" s="9"/>
       <c r="E368" s="9"/>
     </row>
-    <row r="369" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="369" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B369" s="9"/>
       <c r="E369" s="9"/>
     </row>
-    <row r="370" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="370" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B370" s="9"/>
       <c r="E370" s="9"/>
     </row>
-    <row r="371" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="371" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B371" s="9"/>
       <c r="E371" s="9"/>
     </row>
-    <row r="372" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="372" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B372" s="9"/>
       <c r="E372" s="9"/>
     </row>
-    <row r="373" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="373" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B373" s="9"/>
       <c r="E373" s="9"/>
     </row>
-    <row r="374" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="374" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B374" s="9"/>
       <c r="E374" s="9"/>
     </row>
-    <row r="375" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="375" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B375" s="9"/>
       <c r="E375" s="9"/>
     </row>
-    <row r="376" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="376" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B376" s="9"/>
       <c r="E376" s="9"/>
     </row>
-    <row r="377" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="377" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B377" s="9"/>
       <c r="E377" s="9"/>
     </row>
-    <row r="378" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="378" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B378" s="9"/>
       <c r="E378" s="9"/>
     </row>
-    <row r="379" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="379" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B379" s="9"/>
       <c r="E379" s="9"/>
     </row>
-    <row r="380" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="380" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B380" s="9"/>
       <c r="E380" s="9"/>
     </row>
-    <row r="381" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="381" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B381" s="9"/>
       <c r="E381" s="9"/>
     </row>
-    <row r="382" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="382" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B382" s="9"/>
       <c r="E382" s="9"/>
     </row>
-    <row r="383" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="383" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B383" s="9"/>
       <c r="E383" s="9"/>
     </row>
-    <row r="384" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="384" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B384" s="9"/>
       <c r="E384" s="9"/>
     </row>
-    <row r="385" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="385" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B385" s="9"/>
       <c r="E385" s="9"/>
     </row>
-    <row r="386" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="386" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B386" s="9"/>
       <c r="E386" s="9"/>
     </row>
-    <row r="387" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="387" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B387" s="9"/>
       <c r="E387" s="9"/>
     </row>
-    <row r="388" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="388" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B388" s="9"/>
       <c r="E388" s="9"/>
     </row>
-    <row r="389" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="389" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B389" s="9"/>
       <c r="E389" s="9"/>
     </row>
-    <row r="390" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="390" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B390" s="9"/>
       <c r="E390" s="9"/>
     </row>
-    <row r="391" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="391" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B391" s="9"/>
       <c r="E391" s="9"/>
     </row>
-    <row r="392" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="392" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B392" s="9"/>
       <c r="E392" s="9"/>
     </row>
-    <row r="393" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="393" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B393" s="9"/>
       <c r="E393" s="9"/>
     </row>
-    <row r="394" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="394" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B394" s="9"/>
       <c r="E394" s="9"/>
     </row>
-    <row r="395" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="395" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B395" s="9"/>
       <c r="E395" s="9"/>
     </row>
-    <row r="396" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="396" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B396" s="9"/>
       <c r="E396" s="9"/>
     </row>
-    <row r="397" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="397" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B397" s="9"/>
       <c r="E397" s="9"/>
     </row>
-    <row r="398" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="398" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B398" s="9"/>
       <c r="E398" s="9"/>
     </row>
-    <row r="399" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="399" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B399" s="9"/>
       <c r="E399" s="9"/>
     </row>
-    <row r="400" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="400" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B400" s="9"/>
       <c r="E400" s="9"/>
     </row>
-    <row r="401" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="401" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B401" s="9"/>
       <c r="E401" s="9"/>
     </row>
-    <row r="402" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="402" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B402" s="9"/>
       <c r="E402" s="9"/>
     </row>
-    <row r="403" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="403" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B403" s="9"/>
       <c r="E403" s="9"/>
     </row>
-    <row r="404" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="404" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B404" s="9"/>
       <c r="E404" s="9"/>
     </row>
-    <row r="405" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="405" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B405" s="9"/>
       <c r="E405" s="9"/>
     </row>
-    <row r="406" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="406" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B406" s="9"/>
       <c r="E406" s="9"/>
     </row>
-    <row r="407" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="407" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B407" s="9"/>
       <c r="E407" s="9"/>
     </row>
-    <row r="408" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="408" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B408" s="9"/>
       <c r="E408" s="9"/>
     </row>
-    <row r="409" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="409" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B409" s="9"/>
       <c r="E409" s="9"/>
     </row>
-    <row r="410" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="410" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B410" s="9"/>
       <c r="E410" s="9"/>
     </row>
-    <row r="411" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="411" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B411" s="9"/>
       <c r="E411" s="9"/>
     </row>
-    <row r="412" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="412" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B412" s="9"/>
       <c r="E412" s="9"/>
     </row>
-    <row r="413" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="413" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B413" s="9"/>
       <c r="E413" s="9"/>
     </row>
-    <row r="414" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="414" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B414" s="9"/>
       <c r="E414" s="9"/>
     </row>
-    <row r="415" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="415" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B415" s="9"/>
       <c r="E415" s="9"/>
     </row>
-    <row r="416" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="416" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B416" s="9"/>
       <c r="E416" s="9"/>
     </row>
-    <row r="417" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="417" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B417" s="9"/>
       <c r="E417" s="9"/>
     </row>
-    <row r="418" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="418" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B418" s="9"/>
       <c r="E418" s="9"/>
     </row>
-    <row r="419" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="419" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B419" s="9"/>
       <c r="E419" s="9"/>
     </row>
-    <row r="420" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="420" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B420" s="9"/>
       <c r="E420" s="9"/>
     </row>
-    <row r="421" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="421" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B421" s="9"/>
       <c r="E421" s="9"/>
     </row>
-    <row r="422" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="422" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B422" s="9"/>
       <c r="E422" s="9"/>
     </row>
-    <row r="423" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="423" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B423" s="9"/>
       <c r="E423" s="9"/>
     </row>
-    <row r="424" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="424" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B424" s="9"/>
       <c r="E424" s="9"/>
     </row>
-    <row r="425" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="425" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B425" s="9"/>
       <c r="E425" s="9"/>
     </row>
-    <row r="426" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="426" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B426" s="9"/>
       <c r="E426" s="9"/>
     </row>
-    <row r="427" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="427" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B427" s="9"/>
       <c r="E427" s="9"/>
     </row>
-    <row r="428" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="428" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B428" s="9"/>
       <c r="E428" s="9"/>
     </row>
-    <row r="429" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="429" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B429" s="9"/>
       <c r="E429" s="9"/>
     </row>
-    <row r="430" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="430" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B430" s="9"/>
       <c r="E430" s="9"/>
     </row>
-    <row r="431" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="431" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B431" s="9"/>
       <c r="E431" s="9"/>
     </row>
-    <row r="432" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="432" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B432" s="9"/>
       <c r="E432" s="9"/>
     </row>
-    <row r="433" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="433" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B433" s="9"/>
       <c r="E433" s="9"/>
     </row>
-    <row r="434" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="434" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B434" s="9"/>
       <c r="E434" s="9"/>
     </row>
-    <row r="435" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="435" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B435" s="9"/>
       <c r="E435" s="9"/>
     </row>
-    <row r="436" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="436" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B436" s="9"/>
       <c r="E436" s="9"/>
     </row>
-    <row r="437" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="437" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B437" s="9"/>
       <c r="E437" s="9"/>
     </row>
-    <row r="438" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="438" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B438" s="9"/>
       <c r="E438" s="9"/>
     </row>
-    <row r="439" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="439" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B439" s="9"/>
       <c r="E439" s="9"/>
     </row>
-    <row r="440" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="440" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B440" s="9"/>
       <c r="E440" s="9"/>
     </row>
-    <row r="441" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="441" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B441" s="9"/>
       <c r="E441" s="9"/>
     </row>
-    <row r="442" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="442" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B442" s="9"/>
       <c r="E442" s="9"/>
     </row>
-    <row r="443" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="443" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B443" s="9"/>
       <c r="E443" s="9"/>
     </row>
-    <row r="444" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="444" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B444" s="9"/>
       <c r="E444" s="9"/>
     </row>
-    <row r="445" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="445" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B445" s="9"/>
       <c r="E445" s="9"/>
     </row>
-    <row r="446" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="446" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B446" s="9"/>
       <c r="E446" s="9"/>
     </row>
-    <row r="447" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="447" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B447" s="9"/>
       <c r="E447" s="9"/>
     </row>
-    <row r="448" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="448" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B448" s="9"/>
       <c r="E448" s="9"/>
     </row>
-    <row r="449" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="449" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B449" s="9"/>
       <c r="E449" s="9"/>
     </row>
-    <row r="450" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="450" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B450" s="9"/>
       <c r="E450" s="9"/>
     </row>
-    <row r="451" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="451" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B451" s="9"/>
       <c r="E451" s="9"/>
     </row>
-    <row r="452" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="452" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B452" s="9"/>
       <c r="E452" s="9"/>
     </row>
-    <row r="453" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="453" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B453" s="9"/>
       <c r="E453" s="9"/>
     </row>
-    <row r="454" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="454" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B454" s="9"/>
       <c r="E454" s="9"/>
     </row>
-    <row r="455" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="455" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B455" s="9"/>
       <c r="E455" s="9"/>
     </row>
-    <row r="456" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="456" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B456" s="9"/>
       <c r="E456" s="9"/>
     </row>
-    <row r="457" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="457" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B457" s="9"/>
       <c r="E457" s="9"/>
     </row>
-    <row r="458" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="458" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B458" s="9"/>
       <c r="E458" s="9"/>
     </row>
-    <row r="459" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="459" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B459" s="9"/>
       <c r="E459" s="9"/>
     </row>
-    <row r="460" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="460" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B460" s="9"/>
       <c r="E460" s="9"/>
     </row>
-    <row r="461" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="461" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B461" s="9"/>
       <c r="E461" s="9"/>
     </row>
-    <row r="462" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="462" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B462" s="9"/>
       <c r="E462" s="9"/>
     </row>
-    <row r="463" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="463" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B463" s="9"/>
       <c r="E463" s="9"/>
     </row>
-    <row r="464" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="464" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B464" s="9"/>
       <c r="E464" s="9"/>
     </row>
-    <row r="465" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="465" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B465" s="9"/>
       <c r="E465" s="9"/>
     </row>
-    <row r="466" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="466" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B466" s="9"/>
       <c r="E466" s="9"/>
     </row>
-    <row r="467" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="467" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B467" s="9"/>
       <c r="E467" s="9"/>
     </row>
-    <row r="468" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="468" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B468" s="9"/>
       <c r="E468" s="9"/>
     </row>
-    <row r="469" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="469" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B469" s="9"/>
       <c r="E469" s="9"/>
     </row>
-    <row r="470" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="470" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B470" s="9"/>
       <c r="E470" s="9"/>
     </row>
-    <row r="471" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="471" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B471" s="9"/>
       <c r="E471" s="9"/>
     </row>
-    <row r="472" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="472" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B472" s="9"/>
       <c r="E472" s="9"/>
     </row>
-    <row r="473" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="473" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B473" s="9"/>
       <c r="E473" s="9"/>
     </row>
-    <row r="474" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="474" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B474" s="9"/>
       <c r="E474" s="9"/>
     </row>
-    <row r="475" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="475" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B475" s="9"/>
       <c r="E475" s="9"/>
     </row>
-    <row r="476" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="476" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B476" s="9"/>
       <c r="E476" s="9"/>
     </row>
-    <row r="477" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="477" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B477" s="9"/>
       <c r="E477" s="9"/>
     </row>
-    <row r="478" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="478" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B478" s="9"/>
       <c r="E478" s="9"/>
     </row>
-    <row r="479" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="479" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B479" s="9"/>
       <c r="E479" s="9"/>
     </row>
-    <row r="480" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="480" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B480" s="9"/>
       <c r="E480" s="9"/>
     </row>
-    <row r="481" spans="2:5" x14ac:dyDescent="0.45">
+    <row r="481" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B481" s="9"/>
       <c r="E481" s="9"/>
     </row>
@@ -3979,11 +3993,11 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.53125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.53125" style="21"/>
-    <col min="2" max="2" width="23.46484375" style="21" customWidth="1"/>
-    <col min="3" max="16384" width="11.53125" style="21"/>
+    <col min="1" max="1" width="11.5546875" style="21"/>
+    <col min="2" max="2" width="23.44140625" style="21" customWidth="1"/>
+    <col min="3" max="16384" width="11.5546875" style="21"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3998,67 +4012,67 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B3" s="25">
         <v>43672</v>
       </c>
       <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D3" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" s="24" t="s">
-        <v>66</v>
-      </c>
       <c r="F3" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" t="s">
         <v>100</v>
-      </c>
-      <c r="H3" t="s">
-        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -4070,66 +4084,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>105</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>